<commit_message>
writing to excel works
</commit_message>
<xml_diff>
--- a/data/excel/info.xlsx
+++ b/data/excel/info.xlsx
@@ -1,121 +1,64 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\faktura_generator\data\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A54A46-97A4-401E-B11F-0B87CF89DCF4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8220" windowWidth="14400" xWindow="400" yWindow="1950"/>
   </bookViews>
   <sheets>
-    <sheet name="Bedrift" sheetId="1" r:id="rId1"/>
-    <sheet name="Elever" sheetId="2" r:id="rId2"/>
-    <sheet name="Kunder" sheetId="3" r:id="rId3"/>
+    <sheet name="Ark1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Bedrift" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Elever" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Kunder" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Ark11" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
-  <si>
-    <t>Navn</t>
-  </si>
-  <si>
-    <t>Adresse</t>
-  </si>
-  <si>
-    <t>Postnummer</t>
-  </si>
-  <si>
-    <t>Epost</t>
-  </si>
-  <si>
-    <t>Telefon</t>
-  </si>
-  <si>
-    <t>Organisajonsnummer</t>
-  </si>
-  <si>
-    <t>Kontonummer</t>
-  </si>
-  <si>
-    <t>Anna Stray Rongve</t>
-  </si>
-  <si>
-    <t>Hafslundveien 8</t>
-  </si>
-  <si>
-    <t>0373 Oslo</t>
-  </si>
-  <si>
-    <t>anna.stray.rongve@gmail.com</t>
-  </si>
-  <si>
-    <t>93649449</t>
-  </si>
-  <si>
-    <t>1214 05 84906</t>
-  </si>
-  <si>
-    <t>Anette Evensen</t>
-  </si>
-  <si>
-    <t>anetteengerevensen@gmail.com</t>
-  </si>
-  <si>
-    <t>Kikkutveien 4A</t>
-  </si>
-  <si>
-    <t>0491 Oslo</t>
-  </si>
-  <si>
-    <t>info@realfagspesialisten.com</t>
-  </si>
-  <si>
-    <t>Realfagspesialisten</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -151,39 +94,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperkobling" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -471,178 +433,342 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Ark1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="16.08984375" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" customWidth="1"/>
-    <col min="5" max="5" width="27.54296875" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>924881682</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
+    <row r="3">
+      <c r="A3" s="6" t="n"/>
+      <c r="B3" s="6" t="n"/>
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="6" t="n"/>
+      <c r="F3" s="6" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDC10EE7-861D-4CCA-A650-DAB505644CCE}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Ark2">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="2" min="2" style="4" width="16.08984375"/>
+    <col customWidth="1" max="3" min="3" style="4" width="15.08984375"/>
+    <col customWidth="1" max="4" min="4" style="4" width="12.08984375"/>
+    <col customWidth="1" max="5" min="5" style="4" width="27.54296875"/>
+    <col customWidth="1" max="7" min="7" style="4" width="19.1796875"/>
+    <col customWidth="1" max="8" min="8" style="4" width="16"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Navn</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Adresse</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Postnummer</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Epost</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Telefon</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Organisajonsnummer</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Kontonummer</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Anna Stray Rongve</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Hafslundveien 8</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0373 Oslo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>anna.stray.rongve@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>93649449</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>924881682</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1214 05 84906</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Ark3">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Navn</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Epost</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Telefon</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="n"/>
+      <c r="H1" s="5" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Anette Evensen</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>anetteengerevensen@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>95338955</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{0AB0699E-85B2-47DC-B036-BAFEB0E4D7ED}"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727B97DC-F701-48D1-9122-249827B792F2}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Ark4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Navn</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Adresse</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Postnummer</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Epost</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="n"/>
+      <c r="G1" s="5" t="n"/>
+      <c r="H1" s="5" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Realfagspesialisten</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Kikkutveien 4A</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0491 Oslo</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>info@realfagspesialisten.com</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Navn</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>Belop_eks_mva</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>Mvakode</t>
+        </is>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>Kontonummer</t>
+        </is>
+      </c>
+      <c r="E2" s="7" t="inlineStr">
+        <is>
+          <t>Antall</t>
+        </is>
+      </c>
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>Varenummer</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HØY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rewrite to english. Need to fix up create_invoice
</commit_message>
<xml_diff>
--- a/data/excel/info.xlsx
+++ b/data/excel/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna Stray Rongve\Google Drive\Enkeltpersonsforetak\Regnskap\Fakturagenerator\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CED3A6-703D-4F94-A849-5F171BC21EE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039295D5-ADE7-4EC0-A4AE-E15F208167A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1980" windowWidth="21600" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42810" yWindow="8280" windowWidth="14400" windowHeight="7815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>

</xml_diff>